<commit_message>
Create test process result complete
</commit_message>
<xml_diff>
--- a/Connected_Office/Connected Office Test Data.xlsx
+++ b/Connected_Office/Connected Office Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cobus\Documents\UiPath\Connected Office Web Application User Automation Testing Revision 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E5F402-1E5C-4D18-A5F9-5C3A9BCE9CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2721B1E8-2D75-4AD3-99C7-B8CD1C48CA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8055" yWindow="2580" windowWidth="17280" windowHeight="9420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1161,7 +1161,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
@@ -1195,7 +1195,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>0</v>
@@ -1212,7 +1212,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -1246,7 +1246,7 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -1280,7 +1280,7 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -1314,7 +1314,7 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>0</v>
@@ -1331,7 +1331,7 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>0</v>
@@ -1348,7 +1348,7 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>0</v>
@@ -1365,7 +1365,7 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>0</v>
@@ -1416,7 +1416,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>0</v>
@@ -1433,7 +1433,7 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>
@@ -1450,7 +1450,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>0</v>
@@ -1467,7 +1467,7 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>0</v>
@@ -1484,7 +1484,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>0</v>
@@ -1501,7 +1501,7 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>0</v>
@@ -1518,7 +1518,7 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>0</v>
@@ -1535,7 +1535,7 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Create and Read test Passed, Update and Delete process created
</commit_message>
<xml_diff>
--- a/Connected_Office/Connected Office Test Data.xlsx
+++ b/Connected_Office/Connected Office Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cobus\Documents\UiPath\Connected Office Web Application User Automation Testing Revision 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CAE2FB-7CFE-4E58-984F-FD0025CFCDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895324F5-079D-4065-98EB-D598C74A801D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8055" yWindow="2580" windowWidth="17280" windowHeight="9420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="1785" windowWidth="21600" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1127,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>0</v>
@@ -1181,7 +1181,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
@@ -1198,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>0</v>
@@ -1215,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>0</v>
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>0</v>
@@ -1249,7 +1249,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>0</v>
@@ -1266,7 +1266,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
@@ -1283,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>0</v>
@@ -1300,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>0</v>
@@ -1317,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
@@ -1351,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
         <v>0</v>
@@ -1368,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>0</v>
@@ -1385,7 +1385,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
@@ -1402,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
@@ -1419,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
@@ -1453,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
@@ -1470,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
@@ -1487,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
@@ -1504,7 +1504,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
@@ -1521,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
@@ -1538,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Update and Delete test passed for Zones. Publish to orchestrator added
</commit_message>
<xml_diff>
--- a/Connected_Office/Connected Office Test Data.xlsx
+++ b/Connected_Office/Connected Office Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cobus\Documents\UiPath\Connected Office Web Application User Automation Testing Revision 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895324F5-079D-4065-98EB-D598C74A801D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44E0686-2E45-4BAA-9F6F-4035E4BBB520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="1785" windowWidth="21600" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1127,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1167,10 +1167,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1184,10 +1184,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1201,10 +1201,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,10 +1218,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,10 +1235,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,10 +1252,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1269,10 +1269,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1286,10 +1286,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,10 +1303,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>